<commit_message>
updated with county setup
</commit_message>
<xml_diff>
--- a/visuals/label-lookup.xlsx
+++ b/visuals/label-lookup.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\60day-TEMP\christy\explore-race\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CLam\github\exploration-race\visuals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB0AC34-7397-4B4D-942B-CF6A66F4A762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB06CA8D-38C9-4C11-9642-80A72A81E5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E326018A-52AE-46E6-86F0-90BD675909C5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E326018A-52AE-46E6-86F0-90BD675909C5}"/>
   </bookViews>
   <sheets>
     <sheet name="new_labels_20251218" sheetId="5" r:id="rId1"/>
-    <sheet name="detail_mp" sheetId="1" r:id="rId2"/>
-    <sheet name="dichot_mp" sheetId="2" r:id="rId3"/>
-    <sheet name="single_mp" sheetId="3" r:id="rId4"/>
-    <sheet name="all_sp" sheetId="4" r:id="rId5"/>
+    <sheet name="kitsap_new_labels_inprog" sheetId="6" r:id="rId2"/>
+    <sheet name="detail_mp" sheetId="1" r:id="rId3"/>
+    <sheet name="dichot_mp" sheetId="2" r:id="rId4"/>
+    <sheet name="single_mp" sheetId="3" r:id="rId5"/>
+    <sheet name="all_sp" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="116">
   <si>
     <t>Grand Total</t>
   </si>
@@ -331,6 +332,63 @@
   </si>
   <si>
     <t>dichot_cat</t>
+  </si>
+  <si>
+    <t>COUNTY</t>
+  </si>
+  <si>
+    <t>Kitsap</t>
+  </si>
+  <si>
+    <t>American Indian or Alaskan Native</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Black or African American</t>
+  </si>
+  <si>
+    <t>Multirace not incl. Asian &amp; white</t>
+  </si>
+  <si>
+    <t>Multirace Harvard</t>
+  </si>
+  <si>
+    <t>Multirace PSRC</t>
+  </si>
+  <si>
+    <t>Multirace incl. Asian</t>
+  </si>
+  <si>
+    <t>Multirace incl. Asian &amp; white</t>
+  </si>
+  <si>
+    <t>Multirace incl. white</t>
+  </si>
+  <si>
+    <t>Native Hawaiian or Pacific Islander</t>
+  </si>
+  <si>
+    <t>People of color</t>
+  </si>
+  <si>
+    <t>Single race Harvard</t>
+  </si>
+  <si>
+    <t>Single race PSRC</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Regional Example</t>
+  </si>
+  <si>
+    <t>*Kitsap Renter Cost Burden by Hhsize</t>
   </si>
 </sst>
 </file>
@@ -354,7 +412,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -385,6 +443,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -398,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -410,9 +474,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{634EF6B8-D97B-41C4-B3B9-923B3D42BC7C}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,6 +1693,666 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE584834-B345-4677-90CE-4AEC9E9ED1E7}">
+  <dimension ref="A1:I29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="39" customWidth="1"/>
+    <col min="9" max="9" width="47.42578125" customWidth="1"/>
+    <col min="10" max="10" width="36.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" t="str">
+        <f>_xlfn.CONCAT(H2, " ", F2)</f>
+        <v>American Indian or Alaskan Native 1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I26" si="0">_xlfn.CONCAT(H3, " ", F3)</f>
+        <v>Asian 2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>Black or African American 3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>Hispanic or Latino 4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>Multirace not incl. Asian &amp; white 5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>Multirace Harvard 6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>Multirace PSRC 7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>Multirace PSRC 8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H10" t="s">
+        <v>104</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>Multirace PSRC 9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>Multirace incl. Asian 10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" t="s">
+        <v>106</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>Multirace incl. Asian &amp; white 11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>Multirace incl. white 12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>Native Hawaiian or Pacific Islander 13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>People of color 14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>Single race Harvard 15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>98</v>
+      </c>
+      <c r="H17" t="s">
+        <v>111</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>Single race PSRC 16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18">
+        <v>17</v>
+      </c>
+      <c r="G18" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" t="s">
+        <v>111</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>Single race PSRC 17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19">
+        <v>18</v>
+      </c>
+      <c r="G19" t="s">
+        <v>98</v>
+      </c>
+      <c r="H19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>Region 18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>Region 19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>Region 20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22">
+        <v>21</v>
+      </c>
+      <c r="G22" t="s">
+        <v>98</v>
+      </c>
+      <c r="H22" t="s">
+        <v>112</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>Region 21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>98</v>
+      </c>
+      <c r="H23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>Two or More Races 22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24">
+        <v>23</v>
+      </c>
+      <c r="G24" t="s">
+        <v>98</v>
+      </c>
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>Two or More Races 23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25">
+        <v>24</v>
+      </c>
+      <c r="G25" t="s">
+        <v>98</v>
+      </c>
+      <c r="H25" t="s">
+        <v>113</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>White 24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26">
+        <v>25</v>
+      </c>
+      <c r="G26" t="s">
+        <v>98</v>
+      </c>
+      <c r="H26" t="s">
+        <v>113</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>White 25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF40C955-C0C2-4730-BDEB-3D5E4AEE29FE}">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -1922,7 +2647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FB78DD-11F2-4E5B-8C0B-9A940529B04D}">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -2187,7 +2912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04D7F9A-34F4-448F-82C5-F5B8AA2A5763}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -2334,7 +3059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4740A518-0AE4-435E-9931-BA1CF8072EBB}">
   <dimension ref="A1:D17"/>
   <sheetViews>

</xml_diff>